<commit_message>
WAY Corrector - تحديث الملف: 20/01/2026, 19:45:36
</commit_message>
<xml_diff>
--- a/pass.xlsx
+++ b/pass.xlsx
@@ -412,7 +412,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>&amp;&amp;=LZDK&amp;3tvHS=qm</v>
+        <v>&amp;&amp;=LZDK&amp;3</v>
       </c>
       <c r="B2" t="str">
         <v/>
@@ -420,7 +420,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v/>
+        <v>638786</v>
       </c>
       <c r="B3" t="str">
         <v/>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 21/01/2026, 16:27:11
</commit_message>
<xml_diff>
--- a/pass.xlsx
+++ b/pass.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -426,10 +426,26 @@
         <v/>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>679056</v>
+      </c>
+      <c r="B4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>ztuome</v>
+      </c>
+      <c r="B5" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 21/01/2026, 16:28:25
</commit_message>
<xml_diff>
--- a/pass.xlsx
+++ b/pass.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -442,10 +442,18 @@
         <v/>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>468032</v>
+      </c>
+      <c r="B6" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>